<commit_message>
folder staucture change and app api with an add
</commit_message>
<xml_diff>
--- a/api/app_api/end_point_module_wise.xlsx
+++ b/api/app_api/end_point_module_wise.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\api\app_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699EDE72-C236-45BD-909B-648977084CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A7FA4E-05F5-4B6F-80A5-2F75AA4B63EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="end_point" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -129,9 +129,6 @@
     <t>Get - provide all ip (conditional)</t>
   </si>
   <si>
-    <t>Get - provide all server (conditional)</t>
-  </si>
-  <si>
     <t>Get - provide details of a single ip</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>POST - Store All Feedback from the user</t>
+  </si>
+  <si>
+    <t>Get - check (conditional) server's ip exists or not</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -638,79 +638,79 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" t="s">
         <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created test cases for api_signup_username_field, also executed test cases for entervpn
</commit_message>
<xml_diff>
--- a/api/app_api/end_point_module_wise.xlsx
+++ b/api/app_api/end_point_module_wise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\api\app_api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A7FA4E-05F5-4B6F-80A5-2F75AA4B63EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5BFE2-7142-4ACA-A68D-7CEDFBF89A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="end_point" sheetId="1" r:id="rId1"/>
@@ -516,17 +516,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -548,7 +548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -559,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -570,7 +570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -581,7 +581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -592,7 +592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -603,7 +603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
@@ -614,7 +614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -625,7 +625,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -636,7 +636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -647,7 +647,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -658,7 +658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -669,7 +669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -680,7 +680,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -691,7 +691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -702,7 +702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
clean up admin panel login feature...
</commit_message>
<xml_diff>
--- a/api/app_api/end_point_module_wise.xlsx
+++ b/api/app_api/end_point_module_wise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\api\app_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A7FA4E-05F5-4B6F-80A5-2F75AA4B63EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DDE28F-9B8F-4261-B24E-A3B44F9BB0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
created test cases for signup(positive and negative) and step1,2 for fibmashvpn
</commit_message>
<xml_diff>
--- a/api/app_api/end_point_module_wise.xlsx
+++ b/api/app_api/end_point_module_wise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\api\app_api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5BFE2-7142-4ACA-A68D-7CEDFBF89A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD072F6-F918-42E2-A569-8B35DD7C6015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>Modules</t>
   </si>
@@ -48,9 +48,6 @@
     <t>/resend-email-verification</t>
   </si>
   <si>
-    <t>/symlex-login-plain</t>
-  </si>
-  <si>
     <t>POST - Send Email Verification</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>8..</t>
   </si>
   <si>
-    <t>9. Server and IP</t>
-  </si>
-  <si>
     <t>/get_ips</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>12..</t>
   </si>
   <si>
-    <t>13..</t>
-  </si>
-  <si>
     <t>14..</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>Get - Provide Feed Back Keywords and Feed back Emoji Agaist a PIN</t>
   </si>
   <si>
-    <t>15. Feedback</t>
-  </si>
-  <si>
     <t>16..</t>
   </si>
   <si>
@@ -178,13 +166,169 @@
   </si>
   <si>
     <t>Get - check (conditional) server's ip exists or not</t>
+  </si>
+  <si>
+    <t>/symlex-login-encrypted</t>
+  </si>
+  <si>
+    <t>/get-referral-balance-statement</t>
+  </si>
+  <si>
+    <t>/use-referral-reseller</t>
+  </si>
+  <si>
+    <t>9..</t>
+  </si>
+  <si>
+    <t>/getVpnServerData</t>
+  </si>
+  <si>
+    <t>15..</t>
+  </si>
+  <si>
+    <t>/wireguard-user-con</t>
+  </si>
+  <si>
+    <t>/get-iap-page-content</t>
+  </si>
+  <si>
+    <t>/server_current_connection_save</t>
+  </si>
+  <si>
+    <t>/user_session_save</t>
+  </si>
+  <si>
+    <t>/getUsersLoggedInDevices</t>
+  </si>
+  <si>
+    <t>/get-referral-info-reseller</t>
+  </si>
+  <si>
+    <t>/update-ip</t>
+  </si>
+  <si>
+    <t>/remove-user</t>
+  </si>
+  <si>
+    <t>/remove-duplicate-payment</t>
+  </si>
+  <si>
+    <t>/reset_udid</t>
+  </si>
+  <si>
+    <t>/reset-password</t>
+  </si>
+  <si>
+    <t>/purchased-transaction-history</t>
+  </si>
+  <si>
+    <t>/save-player-id</t>
+  </si>
+  <si>
+    <t>/save_contact_email</t>
+  </si>
+  <si>
+    <t>13. Server and IP</t>
+  </si>
+  <si>
+    <t>17..</t>
+  </si>
+  <si>
+    <t>18..</t>
+  </si>
+  <si>
+    <t>19..</t>
+  </si>
+  <si>
+    <t>20..</t>
+  </si>
+  <si>
+    <t>21. Feedback</t>
+  </si>
+  <si>
+    <t>22..</t>
+  </si>
+  <si>
+    <t>23. Remove user</t>
+  </si>
+  <si>
+    <t>24. Remove Duplicate payment</t>
+  </si>
+  <si>
+    <t>25. Reset UDID</t>
+  </si>
+  <si>
+    <t>26. Reset Password</t>
+  </si>
+  <si>
+    <t>27. Resend Email Verification</t>
+  </si>
+  <si>
+    <t>28. Purchased Transaction History</t>
+  </si>
+  <si>
+    <t>29. Save Player ID</t>
+  </si>
+  <si>
+    <t>30. Save contact email</t>
+  </si>
+  <si>
+    <t>31. connection and session</t>
+  </si>
+  <si>
+    <t>32..</t>
+  </si>
+  <si>
+    <t>33..</t>
+  </si>
+  <si>
+    <t>34..</t>
+  </si>
+  <si>
+    <t>35..</t>
+  </si>
+  <si>
+    <t>36..</t>
+  </si>
+  <si>
+    <t>37. what is my ip</t>
+  </si>
+  <si>
+    <t>38. payment(ios)</t>
+  </si>
+  <si>
+    <t>39. payment(android)</t>
+  </si>
+  <si>
+    <t>40. payment(SSL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST- </t>
+  </si>
+  <si>
+    <t>GET-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get- </t>
+  </si>
+  <si>
+    <t>POST-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET- </t>
+  </si>
+  <si>
+    <t>41. guest login</t>
+  </si>
+  <si>
+    <t>42.voucher redeem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +344,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +370,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -224,17 +395,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,15 +703,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="63.7109375" customWidth="1"/>
   </cols>
@@ -539,7 +729,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -550,21 +740,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -572,148 +762,401 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
+      <c r="A11" t="s">
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>28</v>
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
+      <c r="A15" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>46</v>
+      <c r="A19" t="s">
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" display="/get-referral-info-reseller?idReseller4=235&amp;username=rumy.kolpolok@gmail.com&amp;pass=123456" xr:uid="{3FFAC2E0-92B4-4C53-B0F7-4B75D4254F66}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>